<commit_message>
Fleshing out the CSO notebook further
</commit_message>
<xml_diff>
--- a/var_details.xlsx
+++ b/var_details.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,24 +10,20 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DC637C-6CF4-4994-B30B-3A3E56AF00A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="director_data" sheetId="1" r:id="rId1"/>
     <sheet name="teacher_data" sheetId="2" r:id="rId2"/>
     <sheet name="cso_data" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">cso_data!$A$1:$G$61</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">director_data!$A$1:$G$48</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">teacher_data!$A$1:$G$49</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8085" uniqueCount="457">
   <si>
     <t>position</t>
   </si>
@@ -1236,6 +1232,168 @@
   </si>
   <si>
     <t>CSO Data</t>
+  </si>
+  <si>
+    <t>str28</t>
+  </si>
+  <si>
+    <t>str29</t>
+  </si>
+  <si>
+    <t>str321</t>
+  </si>
+  <si>
+    <t>str460</t>
+  </si>
+  <si>
+    <t>str110</t>
+  </si>
+  <si>
+    <t>%28s</t>
+  </si>
+  <si>
+    <t>%29s</t>
+  </si>
+  <si>
+    <t>%321s</t>
+  </si>
+  <si>
+    <t>%460s</t>
+  </si>
+  <si>
+    <t>%110s</t>
+  </si>
+  <si>
+    <t>str18</t>
+  </si>
+  <si>
+    <t>str401</t>
+  </si>
+  <si>
+    <t>str309</t>
+  </si>
+  <si>
+    <t>str355</t>
+  </si>
+  <si>
+    <t>%18s</t>
+  </si>
+  <si>
+    <t>%401s</t>
+  </si>
+  <si>
+    <t>%309s</t>
+  </si>
+  <si>
+    <t>%355s</t>
+  </si>
+  <si>
+    <t>str34</t>
+  </si>
+  <si>
+    <t>str83</t>
+  </si>
+  <si>
+    <t>str188</t>
+  </si>
+  <si>
+    <t>str116</t>
+  </si>
+  <si>
+    <t>str262</t>
+  </si>
+  <si>
+    <t>str251</t>
+  </si>
+  <si>
+    <t>str91</t>
+  </si>
+  <si>
+    <t>%34s</t>
+  </si>
+  <si>
+    <t>%83s</t>
+  </si>
+  <si>
+    <t>%188s</t>
+  </si>
+  <si>
+    <t>%116s</t>
+  </si>
+  <si>
+    <t>%262s</t>
+  </si>
+  <si>
+    <t>%251s</t>
+  </si>
+  <si>
+    <t>%91s</t>
+  </si>
+  <si>
+    <t>str430</t>
+  </si>
+  <si>
+    <t>%430s</t>
+  </si>
+  <si>
+    <t>duplicatecheck</t>
+  </si>
+  <si>
+    <t>str1662</t>
+  </si>
+  <si>
+    <t>%1662s</t>
+  </si>
+  <si>
+    <t>duplicate check</t>
+  </si>
+  <si>
+    <t>str1707</t>
+  </si>
+  <si>
+    <t>%1707s</t>
+  </si>
+  <si>
+    <t>str368</t>
+  </si>
+  <si>
+    <t>str553</t>
+  </si>
+  <si>
+    <t>str367</t>
+  </si>
+  <si>
+    <t>%368s</t>
+  </si>
+  <si>
+    <t>%553s</t>
+  </si>
+  <si>
+    <t>%367s</t>
+  </si>
+  <si>
+    <t>str60</t>
+  </si>
+  <si>
+    <t>str109</t>
+  </si>
+  <si>
+    <t>str244</t>
+  </si>
+  <si>
+    <t>str92</t>
+  </si>
+  <si>
+    <t>%60s</t>
+  </si>
+  <si>
+    <t>%109s</t>
+  </si>
+  <si>
+    <t>%244s</t>
+  </si>
+  <si>
+    <t>%92s</t>
   </si>
 </sst>
 </file>
@@ -1283,8 +1441,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1600,154 +1758,172 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection sqref="A1:G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="23.5703125" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="6.28515625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="9.7109375" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.140625" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="14.85546875" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="56.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>421</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>428</v>
       </c>
       <c r="F3" t="s">
         <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>449</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>453</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
         <v>98</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -1759,130 +1935,130 @@
         <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
         <v>98</v>
       </c>
       <c r="G8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>422</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>429</v>
       </c>
       <c r="F10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
         <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>51</v>
@@ -1897,15 +2073,15 @@
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -1920,15 +2096,15 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -1943,107 +2119,107 @@
         <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>423</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>430</v>
       </c>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
         <v>51</v>
@@ -2058,15 +2234,15 @@
         <v>100</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>51</v>
@@ -2081,15 +2257,15 @@
         <v>100</v>
       </c>
       <c r="G21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
@@ -2104,15 +2280,15 @@
         <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>51</v>
@@ -2127,15 +2303,15 @@
         <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
@@ -2150,61 +2326,61 @@
         <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>424</v>
       </c>
       <c r="D25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>431</v>
       </c>
       <c r="F25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
@@ -2219,130 +2395,130 @@
         <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>450</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>454</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="F30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
         <v>98</v>
       </c>
       <c r="G31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
         <v>51</v>
@@ -2357,15 +2533,15 @@
         <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
         <v>51</v>
@@ -2380,15 +2556,15 @@
         <v>100</v>
       </c>
       <c r="G34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
         <v>51</v>
@@ -2403,15 +2579,15 @@
         <v>100</v>
       </c>
       <c r="G35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
         <v>51</v>
@@ -2426,265 +2602,265 @@
         <v>100</v>
       </c>
       <c r="G36" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>451</v>
       </c>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>455</v>
       </c>
       <c r="F37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G37" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F38" t="s">
         <v>98</v>
       </c>
       <c r="G38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>64</v>
+        <v>425</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>432</v>
       </c>
       <c r="F39" t="s">
         <v>98</v>
       </c>
       <c r="G39" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F40" t="s">
         <v>98</v>
       </c>
       <c r="G40" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="F41" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="D42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="F42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G42" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D43" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F43" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>426</v>
       </c>
       <c r="D44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
+        <v>433</v>
       </c>
       <c r="F44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G44" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F45" t="s">
         <v>98</v>
       </c>
       <c r="G45" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>69</v>
+        <v>452</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>456</v>
       </c>
       <c r="F46" t="s">
         <v>98</v>
       </c>
       <c r="G46" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>437</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>441</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>95</v>
+        <v>442</v>
       </c>
       <c r="F47" t="s">
         <v>98</v>
       </c>
       <c r="G47" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
@@ -2714,7 +2890,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
@@ -2724,95 +2900,113 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="20.85546875" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="12.42578125" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="9.7109375" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.140625" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="10" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="60.140625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="C1" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>408</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>404</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>409</v>
       </c>
       <c r="F3" t="s">
         <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
@@ -2821,21 +3015,21 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>201</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="G5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
@@ -2844,21 +3038,21 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -2873,15 +3067,15 @@
         <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
         <v>51</v>
@@ -2896,15 +3090,15 @@
         <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C9" t="s">
         <v>51</v>
@@ -2919,15 +3113,15 @@
         <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
@@ -2942,61 +3136,61 @@
         <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>443</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>446</v>
       </c>
       <c r="F11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>192</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>202</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
         <v>51</v>
@@ -3011,15 +3205,15 @@
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
@@ -3034,15 +3228,15 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -3057,15 +3251,15 @@
         <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
         <v>51</v>
@@ -3080,15 +3274,15 @@
         <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
         <v>51</v>
@@ -3103,15 +3297,15 @@
         <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
@@ -3126,61 +3320,61 @@
         <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>435</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>436</v>
       </c>
       <c r="F19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C20" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G20" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C21" t="s">
         <v>51</v>
@@ -3195,15 +3389,15 @@
         <v>100</v>
       </c>
       <c r="G21" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
@@ -3218,15 +3412,15 @@
         <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C23" t="s">
         <v>51</v>
@@ -3241,15 +3435,15 @@
         <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C24" t="s">
         <v>51</v>
@@ -3264,15 +3458,15 @@
         <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C25" t="s">
         <v>51</v>
@@ -3287,61 +3481,61 @@
         <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>194</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>204</v>
       </c>
       <c r="F26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G26" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C27" t="s">
-        <v>194</v>
+        <v>51</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>204</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C28" t="s">
         <v>51</v>
@@ -3356,15 +3550,15 @@
         <v>100</v>
       </c>
       <c r="G28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -3379,15 +3573,15 @@
         <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C30" t="s">
         <v>51</v>
@@ -3402,61 +3596,61 @@
         <v>100</v>
       </c>
       <c r="G30" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>444</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>78</v>
+        <v>447</v>
       </c>
       <c r="F31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G31" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G32" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C33" t="s">
         <v>51</v>
@@ -3471,153 +3665,153 @@
         <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>195</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>205</v>
       </c>
       <c r="F34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G34" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C35" t="s">
-        <v>195</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>205</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G35" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>196</v>
       </c>
       <c r="D36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>206</v>
       </c>
       <c r="F36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G36" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C37" t="s">
-        <v>196</v>
+        <v>51</v>
       </c>
       <c r="D37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>206</v>
+        <v>78</v>
       </c>
       <c r="F37" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G37" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="D38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>207</v>
       </c>
       <c r="F38" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G38" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C39" t="s">
-        <v>197</v>
+        <v>51</v>
       </c>
       <c r="D39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>207</v>
+        <v>78</v>
       </c>
       <c r="F39" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G39" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C40" t="s">
         <v>51</v>
@@ -3632,107 +3826,107 @@
         <v>100</v>
       </c>
       <c r="G40" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="D41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="F41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G41" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C42" t="s">
-        <v>198</v>
+        <v>51</v>
       </c>
       <c r="D42" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>208</v>
+        <v>78</v>
       </c>
       <c r="F42" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G42" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>445</v>
       </c>
       <c r="D43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>78</v>
+        <v>448</v>
       </c>
       <c r="F43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G43" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D44" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F44" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G44" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C45" t="s">
         <v>51</v>
@@ -3747,15 +3941,15 @@
         <v>100</v>
       </c>
       <c r="G45" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="46">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
@@ -3770,58 +3964,58 @@
         <v>100</v>
       </c>
       <c r="G46" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="47">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>190</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>407</v>
       </c>
       <c r="D47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>412</v>
       </c>
       <c r="F47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G47" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>437</v>
       </c>
       <c r="C48" t="s">
-        <v>199</v>
+        <v>438</v>
       </c>
       <c r="D48" s="1">
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>209</v>
+        <v>439</v>
       </c>
       <c r="F48" t="s">
         <v>98</v>
       </c>
       <c r="G48" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="49">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
@@ -3851,9 +4045,9 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G61"/>
@@ -3861,95 +4055,113 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="23.42578125" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="6.28515625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="9.7109375" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="7.140625" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="15.140625" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="56.5703125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="D1" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>413</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>417</v>
       </c>
       <c r="F3" t="s">
         <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>255</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
@@ -3958,24 +4170,24 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -3984,21 +4196,21 @@
         <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -4010,61 +4222,61 @@
         <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>309</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>326</v>
       </c>
       <c r="F8" t="s">
         <v>98</v>
       </c>
       <c r="G8" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C9" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>326</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
@@ -4079,15 +4291,15 @@
         <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C11" t="s">
         <v>51</v>
@@ -4102,15 +4314,15 @@
         <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C12" t="s">
         <v>51</v>
@@ -4125,61 +4337,61 @@
         <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>310</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>327</v>
       </c>
       <c r="F13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G13" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>310</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>327</v>
       </c>
       <c r="F14" t="s">
         <v>98</v>
       </c>
       <c r="G14" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s">
         <v>310</v>
@@ -4194,15 +4406,15 @@
         <v>98</v>
       </c>
       <c r="G15" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C16" t="s">
         <v>310</v>
@@ -4217,38 +4429,38 @@
         <v>98</v>
       </c>
       <c r="G16" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>327</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
@@ -4263,15 +4475,15 @@
         <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C19" t="s">
         <v>51</v>
@@ -4286,291 +4498,291 @@
         <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>311</v>
       </c>
       <c r="D20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>328</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G20" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C21" t="s">
-        <v>311</v>
+        <v>414</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>328</v>
+        <v>418</v>
       </c>
       <c r="F21" t="s">
         <v>98</v>
       </c>
       <c r="G21" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C22" t="s">
-        <v>312</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>329</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>313</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>330</v>
       </c>
       <c r="F23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G23" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C24" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F24" t="s">
         <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C25" t="s">
-        <v>314</v>
+        <v>51</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>331</v>
+        <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>315</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>332</v>
       </c>
       <c r="F26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G26" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C27" t="s">
-        <v>315</v>
+        <v>51</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>332</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>415</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>419</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G28" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C29" t="s">
-        <v>316</v>
+        <v>51</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="F29" t="s">
-        <v>98</v>
+        <v>344</v>
       </c>
       <c r="G29" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>317</v>
       </c>
       <c r="D30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F30" t="s">
-        <v>344</v>
+        <v>98</v>
       </c>
       <c r="G30" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C31" t="s">
-        <v>317</v>
+        <v>51</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>335</v>
+        <v>78</v>
       </c>
       <c r="F31" t="s">
         <v>98</v>
       </c>
       <c r="G31" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C32" t="s">
         <v>51</v>
@@ -4582,87 +4794,87 @@
         <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G32" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>318</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>336</v>
       </c>
       <c r="F33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G33" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C34" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="F34" t="s">
         <v>98</v>
       </c>
       <c r="G34" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C35" t="s">
-        <v>319</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>337</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G35" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C36" t="s">
         <v>51</v>
@@ -4677,15 +4889,15 @@
         <v>100</v>
       </c>
       <c r="G36" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C37" t="s">
         <v>51</v>
@@ -4700,15 +4912,15 @@
         <v>100</v>
       </c>
       <c r="G37" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C38" t="s">
         <v>51</v>
@@ -4723,15 +4935,15 @@
         <v>100</v>
       </c>
       <c r="G38" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C39" t="s">
         <v>51</v>
@@ -4746,15 +4958,15 @@
         <v>100</v>
       </c>
       <c r="G39" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C40" t="s">
         <v>51</v>
@@ -4769,15 +4981,15 @@
         <v>100</v>
       </c>
       <c r="G40" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C41" t="s">
         <v>51</v>
@@ -4792,15 +5004,15 @@
         <v>100</v>
       </c>
       <c r="G41" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C42" t="s">
         <v>51</v>
@@ -4815,15 +5027,15 @@
         <v>100</v>
       </c>
       <c r="G42" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C43" t="s">
         <v>51</v>
@@ -4838,15 +5050,15 @@
         <v>100</v>
       </c>
       <c r="G43" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C44" t="s">
         <v>51</v>
@@ -4861,15 +5073,15 @@
         <v>100</v>
       </c>
       <c r="G44" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="45">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C45" t="s">
         <v>51</v>
@@ -4884,15 +5096,15 @@
         <v>100</v>
       </c>
       <c r="G45" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="46">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
@@ -4907,15 +5119,15 @@
         <v>100</v>
       </c>
       <c r="G46" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="47">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C47" t="s">
         <v>51</v>
@@ -4930,328 +5142,305 @@
         <v>100</v>
       </c>
       <c r="G47" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>298</v>
+      </c>
+      <c r="C48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>299</v>
+      </c>
+      <c r="C49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G49" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>300</v>
+      </c>
+      <c r="C50" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" t="s">
+        <v>100</v>
+      </c>
+      <c r="G50" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>301</v>
+      </c>
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" t="s">
+        <v>100</v>
+      </c>
+      <c r="G51" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>302</v>
+      </c>
+      <c r="C52" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>303</v>
+      </c>
+      <c r="C53" t="s">
+        <v>320</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>338</v>
+      </c>
+      <c r="F53" t="s">
+        <v>98</v>
+      </c>
+      <c r="G53" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>304</v>
+      </c>
+      <c r="C54" t="s">
+        <v>321</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>339</v>
+      </c>
+      <c r="F54" t="s">
+        <v>98</v>
+      </c>
+      <c r="G54" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>305</v>
+      </c>
+      <c r="C55" t="s">
+        <v>322</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>340</v>
+      </c>
+      <c r="F55" t="s">
+        <v>98</v>
+      </c>
+      <c r="G55" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>306</v>
+      </c>
+      <c r="C56" t="s">
+        <v>323</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>341</v>
+      </c>
+      <c r="F56" t="s">
+        <v>98</v>
+      </c>
+      <c r="G56" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>307</v>
+      </c>
+      <c r="C57" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>78</v>
+      </c>
+      <c r="F57" t="s">
+        <v>100</v>
+      </c>
+      <c r="G57" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>308</v>
+      </c>
+      <c r="C58" t="s">
+        <v>416</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>420</v>
+      </c>
+      <c r="F58" t="s">
+        <v>98</v>
+      </c>
+      <c r="G58" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
-        <v>297</v>
-      </c>
-      <c r="C48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
-        <v>78</v>
-      </c>
-      <c r="F48" t="s">
-        <v>100</v>
-      </c>
-      <c r="G48" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="1">
+      <c r="C59" t="s">
+        <v>325</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>343</v>
+      </c>
+      <c r="F59" t="s">
+        <v>98</v>
+      </c>
+      <c r="G59" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
-        <v>298</v>
-      </c>
-      <c r="C49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" t="s">
-        <v>78</v>
-      </c>
-      <c r="F49" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="1">
-        <v>48</v>
-      </c>
-      <c r="B50" t="s">
-        <v>299</v>
-      </c>
-      <c r="C50" t="s">
-        <v>51</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
-        <v>78</v>
-      </c>
-      <c r="F50" t="s">
-        <v>100</v>
-      </c>
-      <c r="G50" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
-        <v>300</v>
-      </c>
-      <c r="C51" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="1">
-        <v>1</v>
-      </c>
-      <c r="E51" t="s">
-        <v>78</v>
-      </c>
-      <c r="F51" t="s">
-        <v>100</v>
-      </c>
-      <c r="G51" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="1">
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
-        <v>301</v>
-      </c>
-      <c r="C52" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1</v>
-      </c>
-      <c r="E52" t="s">
-        <v>78</v>
-      </c>
-      <c r="F52" t="s">
-        <v>100</v>
-      </c>
-      <c r="G52" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="1">
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
-        <v>302</v>
-      </c>
-      <c r="C53" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
-        <v>78</v>
-      </c>
-      <c r="F53" t="s">
-        <v>100</v>
-      </c>
-      <c r="G53" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="1">
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
-        <v>303</v>
-      </c>
-      <c r="C54" t="s">
-        <v>320</v>
-      </c>
-      <c r="D54" s="1">
-        <v>0</v>
-      </c>
-      <c r="E54" t="s">
-        <v>338</v>
-      </c>
-      <c r="F54" t="s">
-        <v>98</v>
-      </c>
-      <c r="G54" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="1">
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>304</v>
-      </c>
-      <c r="C55" t="s">
-        <v>321</v>
-      </c>
-      <c r="D55" s="1">
-        <v>0</v>
-      </c>
-      <c r="E55" t="s">
-        <v>339</v>
-      </c>
-      <c r="F55" t="s">
-        <v>98</v>
-      </c>
-      <c r="G55" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>305</v>
-      </c>
-      <c r="C56" t="s">
-        <v>322</v>
-      </c>
-      <c r="D56" s="1">
-        <v>0</v>
-      </c>
-      <c r="E56" t="s">
-        <v>340</v>
-      </c>
-      <c r="F56" t="s">
-        <v>98</v>
-      </c>
-      <c r="G56" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>306</v>
-      </c>
-      <c r="C57" t="s">
-        <v>323</v>
-      </c>
-      <c r="D57" s="1">
-        <v>0</v>
-      </c>
-      <c r="E57" t="s">
-        <v>341</v>
-      </c>
-      <c r="F57" t="s">
-        <v>98</v>
-      </c>
-      <c r="G57" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="1">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>307</v>
-      </c>
-      <c r="C58" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" s="1">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>78</v>
-      </c>
-      <c r="F58" t="s">
-        <v>100</v>
-      </c>
-      <c r="G58" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>308</v>
-      </c>
-      <c r="C59" t="s">
-        <v>324</v>
-      </c>
-      <c r="D59" s="1">
-        <v>0</v>
-      </c>
-      <c r="E59" t="s">
-        <v>342</v>
-      </c>
-      <c r="F59" t="s">
-        <v>98</v>
-      </c>
-      <c r="G59" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="1">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>46</v>
-      </c>
       <c r="C60" t="s">
-        <v>325</v>
+        <v>71</v>
       </c>
       <c r="D60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>343</v>
+        <v>96</v>
       </c>
       <c r="F60" t="s">
         <v>98</v>
       </c>
       <c r="G60" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="1">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" t="s">
-        <v>71</v>
-      </c>
-      <c r="D61" s="1">
-        <v>1</v>
-      </c>
-      <c r="E61" t="s">
-        <v>96</v>
-      </c>
-      <c r="F61" t="s">
-        <v>98</v>
-      </c>
-      <c r="G61" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Datasets refreshed as of 2018-10-20
</commit_message>
<xml_diff>
--- a/var_details.xlsx
+++ b/var_details.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8876" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9667" uniqueCount="463">
   <si>
     <t>position</t>
   </si>
@@ -1394,6 +1394,24 @@
   </si>
   <si>
     <t>%92s</t>
+  </si>
+  <si>
+    <t>str100</t>
+  </si>
+  <si>
+    <t>str504</t>
+  </si>
+  <si>
+    <t>str436</t>
+  </si>
+  <si>
+    <t>%100s</t>
+  </si>
+  <si>
+    <t>%504s</t>
+  </si>
+  <si>
+    <t>%436s</t>
   </si>
 </sst>
 </file>
@@ -1992,13 +2010,13 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>422</v>
+        <v>457</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>429</v>
+        <v>460</v>
       </c>
       <c r="F10" t="s">
         <v>98</v>
@@ -2452,13 +2470,13 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>458</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>461</v>
       </c>
       <c r="F30" t="s">
         <v>98</v>
@@ -2682,13 +2700,13 @@
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>459</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>91</v>
+        <v>462</v>
       </c>
       <c r="F40" t="s">
         <v>98</v>
@@ -2774,13 +2792,13 @@
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>426</v>
+        <v>322</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>433</v>
+        <v>340</v>
       </c>
       <c r="F44" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Updated .dta files, improved literate programming cells
</commit_message>
<xml_diff>
--- a/var_details.xlsx
+++ b/var_details.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9667" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12594" uniqueCount="475">
   <si>
     <t>position</t>
   </si>
@@ -1412,6 +1412,42 @@
   </si>
   <si>
     <t>%436s</t>
+  </si>
+  <si>
+    <t>str19</t>
+  </si>
+  <si>
+    <t>%19s</t>
+  </si>
+  <si>
+    <t>subcounty</t>
+  </si>
+  <si>
+    <t>str562</t>
+  </si>
+  <si>
+    <t>str127</t>
+  </si>
+  <si>
+    <t>%562s</t>
+  </si>
+  <si>
+    <t>%127s</t>
+  </si>
+  <si>
+    <t>Subcounty</t>
+  </si>
+  <si>
+    <t>strL</t>
+  </si>
+  <si>
+    <t>%9s</t>
+  </si>
+  <si>
+    <t>str38</t>
+  </si>
+  <si>
+    <t>%38s</t>
   </si>
 </sst>
 </file>
@@ -1846,22 +1882,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>465</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>473</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>428</v>
+        <v>474</v>
       </c>
       <c r="F3" t="s">
         <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4">
@@ -1964,13 +2000,13 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>466</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>468</v>
       </c>
       <c r="F8" t="s">
         <v>98</v>
@@ -2010,13 +2046,13 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="F10" t="s">
         <v>98</v>
@@ -2861,13 +2897,13 @@
         <v>437</v>
       </c>
       <c r="C47" t="s">
-        <v>441</v>
+        <v>471</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>442</v>
+        <v>472</v>
       </c>
       <c r="F47" t="s">
         <v>98</v>
@@ -4065,7 +4101,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G61"/>
@@ -4136,13 +4172,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>413</v>
+        <v>463</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>417</v>
+        <v>464</v>
       </c>
       <c r="F3" t="s">
         <v>98</v>
@@ -5444,21 +5480,44 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>437</v>
+      </c>
+      <c r="C60" t="s">
+        <v>471</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>472</v>
+      </c>
+      <c r="F60" t="s">
+        <v>98</v>
+      </c>
+      <c r="G60" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>47</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
         <v>96</v>
       </c>
-      <c r="F60" t="s">
-        <v>98</v>
-      </c>
-      <c r="G60" t="s">
+      <c r="F61" t="s">
+        <v>98</v>
+      </c>
+      <c r="G61" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rescuing 'complete teacher' NB, cleaning up deleted files
</commit_message>
<xml_diff>
--- a/var_details.xlsx
+++ b/var_details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="414">
   <si>
     <t>position</t>
   </si>
@@ -1245,6 +1245,18 @@
   </si>
   <si>
     <t>Desired TangDB revisions</t>
+  </si>
+  <si>
+    <t>str144</t>
+  </si>
+  <si>
+    <t>str464</t>
+  </si>
+  <si>
+    <t>%144s</t>
+  </si>
+  <si>
+    <t>%464s</t>
   </si>
 </sst>
 </file>
@@ -4240,13 +4252,13 @@
         <v>305</v>
       </c>
       <c r="C18" t="s">
-        <v>339</v>
+        <v>410</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>356</v>
+        <v>412</v>
       </c>
       <c r="F18" t="s">
         <v>85</v>
@@ -4792,13 +4804,13 @@
         <v>329</v>
       </c>
       <c r="C42" t="s">
-        <v>348</v>
+        <v>411</v>
       </c>
       <c r="D42" s="1">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>365</v>
+        <v>413</v>
       </c>
       <c r="F42" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
Updated for Carmen Sat morning
</commit_message>
<xml_diff>
--- a/var_details.xlsx
+++ b/var_details.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4776" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11698" uniqueCount="416">
   <si>
     <t>position</t>
   </si>
@@ -1257,6 +1257,12 @@
   </si>
   <si>
     <t>%464s</t>
+  </si>
+  <si>
+    <t>%44.0g</t>
+  </si>
+  <si>
+    <t>%51.0g</t>
   </si>
 </sst>
 </file>
@@ -2524,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>214</v>
+        <v>415</v>
       </c>
       <c r="F4" t="s">
         <v>233</v>
@@ -3936,7 +3942,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>214</v>
+        <v>415</v>
       </c>
       <c r="F4" t="s">
         <v>233</v>

</xml_diff>